<commit_message>
Updated with 8keyRelayModule firmware files
</commit_message>
<xml_diff>
--- a/Hardware/BOM/CompInStock.xlsx
+++ b/Hardware/BOM/CompInStock.xlsx
@@ -843,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:I106"/>
+  <dimension ref="A5:I109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2289,6 +2289,11 @@
         <v>2.9</v>
       </c>
     </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="4">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>